<commit_message>
Added proper tables for all results
</commit_message>
<xml_diff>
--- a/data/Risk_free.xlsx
+++ b/data/Risk_free.xlsx
@@ -396,7 +396,7 @@
         <v>32875</v>
       </c>
       <c r="B2">
-        <v>0.01985731784407869</v>
+        <v>0.6525</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -404,7 +404,7 @@
         <v>32905</v>
       </c>
       <c r="B3">
-        <v>0.02001665279703581</v>
+        <v>0.6683333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -412,7 +412,7 @@
         <v>32933</v>
       </c>
       <c r="B4">
-        <v>0.02006644567084178</v>
+        <v>0.6733333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -420,7 +420,7 @@
         <v>32965</v>
       </c>
       <c r="B5">
-        <v>0.02004158016126915</v>
+        <v>0.6708333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -428,7 +428,7 @@
         <v>32994</v>
       </c>
       <c r="B6">
-        <v>0.02015709614259344</v>
+        <v>0.6825</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -436,7 +436,7 @@
         <v>33025</v>
       </c>
       <c r="B7">
-        <v>0.01994987447654809</v>
+        <v>0.6616666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -444,7 +444,7 @@
         <v>33056</v>
       </c>
       <c r="B8">
-        <v>0.02</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -452,7 +452,7 @@
         <v>33086</v>
       </c>
       <c r="B9">
-        <v>0.0197211296389012</v>
+        <v>0.6391666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -460,7 +460,7 @@
         <v>33120</v>
       </c>
       <c r="B10">
-        <v>0.01969538400957933</v>
+        <v>0.6366666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -468,7 +468,7 @@
         <v>33147</v>
       </c>
       <c r="B11">
-        <v>0.01946058221889106</v>
+        <v>0.6141666666666666</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -476,7 +476,7 @@
         <v>33178</v>
       </c>
       <c r="B12">
-        <v>0.019381042166867</v>
+        <v>0.6066666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -484,7 +484,7 @@
         <v>33210</v>
       </c>
       <c r="B13">
-        <v>0.019381042166867</v>
+        <v>0.6066666666666667</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -492,7 +492,7 @@
         <v>33240</v>
       </c>
       <c r="B14">
-        <v>0.01881444491174097</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -500,7 +500,7 @@
         <v>33270</v>
       </c>
       <c r="B15">
-        <v>0.01834122708739614</v>
+        <v>0.5141666666666667</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -508,7 +508,7 @@
         <v>33298</v>
       </c>
       <c r="B16">
-        <v>0.01843978474032827</v>
+        <v>0.5225</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -516,7 +516,7 @@
         <v>33329</v>
       </c>
       <c r="B17">
-        <v>0.01811043221039306</v>
+        <v>0.4950000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -524,7 +524,7 @@
         <v>33359</v>
       </c>
       <c r="B18">
-        <v>0.01787360006641064</v>
+        <v>0.4758333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -532,7 +532,7 @@
         <v>33392</v>
       </c>
       <c r="B19">
-        <v>0.01795668597903639</v>
+        <v>0.4825</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -540,7 +540,7 @@
         <v>33420</v>
       </c>
       <c r="B20">
-        <v>0.01792561898622866</v>
+        <v>0.4799999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -548,7 +548,7 @@
         <v>33451</v>
       </c>
       <c r="B21">
-        <v>0.01788402807348255</v>
+        <v>0.4766666666666666</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -556,7 +556,7 @@
         <v>33484</v>
       </c>
       <c r="B22">
-        <v>0.01766243322477842</v>
+        <v>0.4591666666666666</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -564,7 +564,7 @@
         <v>33512</v>
       </c>
       <c r="B23">
-        <v>0.01738013322443225</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -572,7 +572,7 @@
         <v>33543</v>
       </c>
       <c r="B24">
-        <v>0.01697343023666491</v>
+        <v>0.4075</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -580,7 +580,7 @@
         <v>33574</v>
       </c>
       <c r="B25">
-        <v>0.01652185655703605</v>
+        <v>0.3758333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -588,7 +588,7 @@
         <v>33605</v>
       </c>
       <c r="B26">
-        <v>0.0158209197869304</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -596,7 +596,7 @@
         <v>33637</v>
       </c>
       <c r="B27">
-        <v>0.0158209197869304</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -604,7 +604,7 @@
         <v>33665</v>
       </c>
       <c r="B28">
-        <v>0.0160570877363124</v>
+        <v>0.345</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -612,7 +612,7 @@
         <v>33695</v>
       </c>
       <c r="B29">
-        <v>0.01601820843710718</v>
+        <v>0.3425</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -620,7 +620,7 @@
         <v>33725</v>
       </c>
       <c r="B30">
-        <v>0.01549462178999157</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -628,7 +628,7 @@
         <v>33756</v>
       </c>
       <c r="B31">
-        <v>0.01563223664786194</v>
+        <v>0.3183333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -636,7 +636,7 @@
         <v>33786</v>
       </c>
       <c r="B32">
-        <v>0.01536864368095257</v>
+        <v>0.3025</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -644,7 +644,7 @@
         <v>33819</v>
       </c>
       <c r="B33">
-        <v>0.01481248034203685</v>
+        <v>0.2708333333333333</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -652,7 +652,7 @@
         <v>33848</v>
       </c>
       <c r="B34">
-        <v>0.01476676251932837</v>
+        <v>0.2683333333333334</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -660,7 +660,7 @@
         <v>33878</v>
       </c>
       <c r="B35">
-        <v>0.01387300109179834</v>
+        <v>0.2225</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -668,7 +668,7 @@
         <v>33910</v>
       </c>
       <c r="B36">
-        <v>0.01454957269758291</v>
+        <v>0.2566666666666667</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -676,7 +676,7 @@
         <v>33939</v>
       </c>
       <c r="B37">
-        <v>0.01503694596204975</v>
+        <v>0.2833333333333333</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -684,7 +684,7 @@
         <v>33973</v>
       </c>
       <c r="B38">
-        <v>0.01472075984577927</v>
+        <v>0.2658333333333334</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -692,7 +692,7 @@
         <v>34001</v>
       </c>
       <c r="B39">
-        <v>0.01443850292564962</v>
+        <v>0.2508333333333334</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -700,7 +700,7 @@
         <v>34029</v>
       </c>
       <c r="B40">
-        <v>0.01447041132318426</v>
+        <v>0.2525</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -708,7 +708,7 @@
         <v>34060</v>
       </c>
       <c r="B41">
-        <v>0.01435810870413664</v>
+        <v>0.2466666666666666</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -716,7 +716,7 @@
         <v>34092</v>
       </c>
       <c r="B42">
-        <v>0.01430943677571399</v>
+        <v>0.2441666666666667</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -724,7 +724,7 @@
         <v>34121</v>
       </c>
       <c r="B43">
-        <v>0.01464344350503119</v>
+        <v>0.2616666666666667</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -732,7 +732,7 @@
         <v>34151</v>
       </c>
       <c r="B44">
-        <v>0.01451801170324752</v>
+        <v>0.255</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -740,7 +740,7 @@
         <v>34183</v>
       </c>
       <c r="B45">
-        <v>0.01468993093911307</v>
+        <v>0.2641666666666667</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -748,7 +748,7 @@
         <v>34213</v>
       </c>
       <c r="B46">
-        <v>0.01454957269758291</v>
+        <v>0.2566666666666667</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -756,7 +756,7 @@
         <v>34243</v>
       </c>
       <c r="B47">
-        <v>0.01439037422545773</v>
+        <v>0.2483333333333334</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -764,7 +764,7 @@
         <v>34274</v>
       </c>
       <c r="B48">
-        <v>0.01470536155018365</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -772,7 +772,7 @@
         <v>34304</v>
       </c>
       <c r="B49">
-        <v>0.01472075984577927</v>
+        <v>0.2658333333333334</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -780,7 +780,7 @@
         <v>34337</v>
       </c>
       <c r="B50">
-        <v>0.01467446784248556</v>
+        <v>0.2633333333333334</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -788,7 +788,7 @@
         <v>34366</v>
       </c>
       <c r="B51">
-        <v>0.01458099735826712</v>
+        <v>0.2583333333333334</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -796,7 +796,7 @@
         <v>34394</v>
       </c>
       <c r="B52">
-        <v>0.01529775409527345</v>
+        <v>0.2983333333333333</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -804,7 +804,7 @@
         <v>34428</v>
       </c>
       <c r="B53">
-        <v>0.01563223664786194</v>
+        <v>0.3183333333333333</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -812,7 +812,7 @@
         <v>34456</v>
       </c>
       <c r="B54">
-        <v>0.01600520663883155</v>
+        <v>0.3416666666666666</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -820,7 +820,7 @@
         <v>34486</v>
       </c>
       <c r="B55">
-        <v>0.01623608275859847</v>
+        <v>0.3566666666666667</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -828,7 +828,7 @@
         <v>34516</v>
       </c>
       <c r="B56">
-        <v>0.01628650569956944</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -836,7 +836,7 @@
         <v>34547</v>
       </c>
       <c r="B57">
-        <v>0.01644826156553362</v>
+        <v>0.3708333333333333</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -844,7 +844,7 @@
         <v>34578</v>
       </c>
       <c r="B58">
-        <v>0.01671497097747405</v>
+        <v>0.3891666666666667</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -852,7 +852,7 @@
         <v>34610</v>
       </c>
       <c r="B59">
-        <v>0.01715656971621709</v>
+        <v>0.4208333333333333</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -860,7 +860,7 @@
         <v>34639</v>
       </c>
       <c r="B60">
-        <v>0.01734696495064666</v>
+        <v>0.435</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -868,7 +868,7 @@
         <v>34669</v>
       </c>
       <c r="B61">
-        <v>0.01787360006641064</v>
+        <v>0.4758333333333334</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -876,7 +876,7 @@
         <v>34702</v>
       </c>
       <c r="B62">
-        <v>0.01812058949362758</v>
+        <v>0.4958333333333333</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -884,7 +884,7 @@
         <v>34731</v>
       </c>
       <c r="B63">
-        <v>0.01824159868515518</v>
+        <v>0.5058333333333334</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -892,7 +892,7 @@
         <v>34759</v>
       </c>
       <c r="B64">
-        <v>0.01811043221039306</v>
+        <v>0.4950000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -900,7 +900,7 @@
         <v>34792</v>
       </c>
       <c r="B65">
-        <v>0.01811043221039306</v>
+        <v>0.4950000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -908,7 +908,7 @@
         <v>34820</v>
       </c>
       <c r="B66">
-        <v>0.01807989179458566</v>
+        <v>0.4925</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -916,7 +916,7 @@
         <v>34851</v>
       </c>
       <c r="B67">
-        <v>0.01783176585828939</v>
+        <v>0.4725</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -924,7 +924,7 @@
         <v>34883</v>
       </c>
       <c r="B68">
-        <v>0.01784224280891269</v>
+        <v>0.4733333333333333</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -932,7 +932,7 @@
         <v>34912</v>
       </c>
       <c r="B69">
-        <v>0.01776864403498478</v>
+        <v>0.4675</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -940,7 +940,7 @@
         <v>34943</v>
       </c>
       <c r="B70">
-        <v>0.01759808863540803</v>
+        <v>0.4541666666666667</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -948,7 +948,7 @@
         <v>34974</v>
       </c>
       <c r="B71">
-        <v>0.01768377757572738</v>
+        <v>0.4608333333333334</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -956,7 +956,7 @@
         <v>35004</v>
       </c>
       <c r="B72">
-        <v>0.017630319638986</v>
+        <v>0.4566666666666667</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -964,7 +964,7 @@
         <v>35034</v>
       </c>
       <c r="B73">
-        <v>0.01759808863540803</v>
+        <v>0.4541666666666667</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -972,7 +972,7 @@
         <v>35066</v>
       </c>
       <c r="B74">
-        <v>0.01732478210681805</v>
+        <v>0.4333333333333333</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -980,7 +980,7 @@
         <v>35096</v>
       </c>
       <c r="B75">
-        <v>0.01713389081375144</v>
+        <v>0.4191666666666667</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -988,7 +988,7 @@
         <v>35125</v>
       </c>
       <c r="B76">
-        <v>0.01707692932017028</v>
+        <v>0.415</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -996,7 +996,7 @@
         <v>35156</v>
       </c>
       <c r="B77">
-        <v>0.01732478210681805</v>
+        <v>0.4333333333333333</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1004,7 +1004,7 @@
         <v>35186</v>
       </c>
       <c r="B78">
-        <v>0.01722424919295968</v>
+        <v>0.4258333333333333</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1012,7 +1012,7 @@
         <v>35219</v>
       </c>
       <c r="B79">
-        <v>0.01735803512911434</v>
+        <v>0.4358333333333334</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1020,7 +1020,7 @@
         <v>35247</v>
       </c>
       <c r="B80">
-        <v>0.0174021752686287</v>
+        <v>0.4391666666666666</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>35278</v>
       </c>
       <c r="B81">
-        <v>0.01738013322443225</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>35311</v>
       </c>
       <c r="B82">
-        <v>0.01745703747037208</v>
+        <v>0.4433333333333334</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>35339</v>
       </c>
       <c r="B83">
-        <v>0.01721300620726316</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>35370</v>
       </c>
       <c r="B84">
-        <v>0.01729140094106259</v>
+        <v>0.4308333333333333</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1060,7 +1060,7 @@
         <v>35401</v>
       </c>
       <c r="B85">
-        <v>0.01719047606867682</v>
+        <v>0.4233333333333333</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>35432</v>
       </c>
       <c r="B86">
-        <v>0.01731366935065357</v>
+        <v>0.4325000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>35464</v>
       </c>
       <c r="B87">
-        <v>0.01723547752025507</v>
+        <v>0.4266666666666666</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>35492</v>
       </c>
       <c r="B88">
-        <v>0.01736909120543431</v>
+        <v>0.4366666666666667</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>35521</v>
       </c>
       <c r="B89">
-        <v>0.01745703747037208</v>
+        <v>0.4433333333333334</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>35551</v>
       </c>
       <c r="B90">
-        <v>0.01736909120543431</v>
+        <v>0.4366666666666667</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>35583</v>
       </c>
       <c r="B91">
-        <v>0.01717918881916198</v>
+        <v>0.4225</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>35612</v>
       </c>
       <c r="B92">
-        <v>0.01730254231073098</v>
+        <v>0.4316666666666666</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1124,7 +1124,7 @@
         <v>35643</v>
       </c>
       <c r="B93">
-        <v>0.01741317538234722</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1132,7 +1132,7 @@
         <v>35675</v>
       </c>
       <c r="B94">
-        <v>0.01733588062497643</v>
+        <v>0.4341666666666667</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1140,7 +1140,7 @@
         <v>35704</v>
       </c>
       <c r="B95">
-        <v>0.01721300620726316</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1148,7 +1148,7 @@
         <v>35737</v>
       </c>
       <c r="B96">
-        <v>0.01739116123070632</v>
+        <v>0.4383333333333333</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>35765</v>
       </c>
       <c r="B97">
-        <v>0.0174021752686287</v>
+        <v>0.4391666666666666</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>35797</v>
       </c>
       <c r="B98">
-        <v>0.01745703747037208</v>
+        <v>0.4433333333333334</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1172,7 +1172,7 @@
         <v>35828</v>
       </c>
       <c r="B99">
-        <v>0.01739116123070632</v>
+        <v>0.4383333333333333</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>35856</v>
       </c>
       <c r="B100">
-        <v>0.01739116123070632</v>
+        <v>0.4383333333333333</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1188,7 +1188,7 @@
         <v>35886</v>
       </c>
       <c r="B101">
-        <v>0.01723547752025507</v>
+        <v>0.4266666666666666</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1196,7 +1196,7 @@
         <v>35916</v>
       </c>
       <c r="B102">
-        <v>0.01712252881385859</v>
+        <v>0.4183333333333333</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>35947</v>
       </c>
       <c r="B103">
-        <v>0.01719047606867682</v>
+        <v>0.4233333333333333</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>35977</v>
       </c>
       <c r="B104">
-        <v>0.01720174851523086</v>
+        <v>0.4241666666666666</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1220,7 +1220,7 @@
         <v>36010</v>
       </c>
       <c r="B105">
-        <v>0.01724669123683449</v>
+        <v>0.4275</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1228,7 +1228,7 @@
         <v>36039</v>
       </c>
       <c r="B106">
-        <v>0.01700806998629276</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1236,7 +1236,7 @@
         <v>36069</v>
       </c>
       <c r="B107">
-        <v>0.01617261032503283</v>
+        <v>0.3525</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1244,7 +1244,7 @@
         <v>36101</v>
       </c>
       <c r="B108">
-        <v>0.01655840945617421</v>
+        <v>0.3783333333333333</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1252,7 +1252,7 @@
         <v>36130</v>
       </c>
       <c r="B109">
-        <v>0.01649739781430644</v>
+        <v>0.3741666666666667</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1260,7 +1260,7 @@
         <v>36164</v>
       </c>
       <c r="B110">
-        <v>0.01649739781430644</v>
+        <v>0.3741666666666667</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1268,7 +1268,7 @@
         <v>36192</v>
       </c>
       <c r="B111">
-        <v>0.01654624309657253</v>
+        <v>0.3775</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1276,7 +1276,7 @@
         <v>36220</v>
       </c>
       <c r="B112">
-        <v>0.01676255834023429</v>
+        <v>0.3925</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1284,7 +1284,7 @@
         <v>36251</v>
       </c>
       <c r="B113">
-        <v>0.01643593152975417</v>
+        <v>0.3700000000000001</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1292,7 +1292,7 @@
         <v>36283</v>
       </c>
       <c r="B114">
-        <v>0.01665510308998826</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1300,7 +1300,7 @@
         <v>36312</v>
       </c>
       <c r="B115">
-        <v>0.01683343680839137</v>
+        <v>0.3975</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1308,7 +1308,7 @@
         <v>36342</v>
       </c>
       <c r="B116">
-        <v>0.01672689321473839</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1316,7 +1316,7 @@
         <v>36374</v>
       </c>
       <c r="B117">
-        <v>0.01692702281372182</v>
+        <v>0.4041666666666667</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1324,7 +1324,7 @@
         <v>36404</v>
       </c>
       <c r="B118">
-        <v>0.01706549131988276</v>
+        <v>0.4141666666666666</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1332,7 +1332,7 @@
         <v>36434</v>
       </c>
       <c r="B119">
-        <v>0.01696185217697622</v>
+        <v>0.4066666666666667</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1340,7 +1340,7 @@
         <v>36465</v>
       </c>
       <c r="B120">
-        <v>0.01728024519542338</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1348,7 +1348,7 @@
         <v>36495</v>
       </c>
       <c r="B121">
-        <v>0.0174021752686287</v>
+        <v>0.4391666666666666</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1356,7 +1356,7 @@
         <v>36528</v>
       </c>
       <c r="B122">
-        <v>0.017630319638986</v>
+        <v>0.4566666666666667</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1364,7 +1364,7 @@
         <v>36557</v>
       </c>
       <c r="B123">
-        <v>0.01787360006641064</v>
+        <v>0.4758333333333334</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1372,7 +1372,7 @@
         <v>36586</v>
       </c>
       <c r="B124">
-        <v>0.01792561898622866</v>
+        <v>0.4799999999999999</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1380,7 +1380,7 @@
         <v>36619</v>
       </c>
       <c r="B125">
-        <v>0.0180390100455943</v>
+        <v>0.4891666666666666</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1388,7 +1388,7 @@
         <v>36647</v>
       </c>
       <c r="B126">
-        <v>0.0181712059283214</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1396,7 +1396,7 @@
         <v>36678</v>
       </c>
       <c r="B127">
-        <v>0.01790484768258862</v>
+        <v>0.4783333333333334</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1404,7 +1404,7 @@
         <v>36710</v>
       </c>
       <c r="B128">
-        <v>0.0181712059283214</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1412,7 +1412,7 @@
         <v>36739</v>
       </c>
       <c r="B129">
-        <v>0.01842015749320193</v>
+        <v>0.5208333333333334</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1420,7 +1420,7 @@
         <v>36770</v>
       </c>
       <c r="B130">
-        <v>0.01843978474032827</v>
+        <v>0.5225</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1428,7 +1428,7 @@
         <v>36801</v>
       </c>
       <c r="B131">
-        <v>0.01843978474032827</v>
+        <v>0.5225</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1436,7 +1436,7 @@
         <v>36831</v>
       </c>
       <c r="B132">
-        <v>0.01853729995781322</v>
+        <v>0.5308333333333333</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1444,7 +1444,7 @@
         <v>36861</v>
       </c>
       <c r="B133">
-        <v>0.0184004883298249</v>
+        <v>0.5191666666666667</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1452,7 +1452,7 @@
         <v>36893</v>
       </c>
       <c r="B134">
-        <v>0.0180390100455943</v>
+        <v>0.4891666666666666</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1460,7 +1460,7 @@
         <v>36923</v>
       </c>
       <c r="B135">
-        <v>0.01709975946676697</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1468,7 +1468,7 @@
         <v>36951</v>
       </c>
       <c r="B136">
-        <v>0.01691538111622984</v>
+        <v>0.4033333333333333</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1476,7 +1476,7 @@
         <v>36983</v>
       </c>
       <c r="B137">
-        <v>0.0161598558951957</v>
+        <v>0.3516666666666666</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1484,7 +1484,7 @@
         <v>37012</v>
       </c>
       <c r="B138">
-        <v>0.01576747032621048</v>
+        <v>0.3266666666666667</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1492,7 +1492,7 @@
         <v>37043</v>
       </c>
       <c r="B139">
-        <v>0.01542488807493123</v>
+        <v>0.3058333333333333</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1500,7 +1500,7 @@
         <v>37074</v>
       </c>
       <c r="B140">
-        <v>0.01542488807493123</v>
+        <v>0.3058333333333333</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1508,7 +1508,7 @@
         <v>37104</v>
       </c>
       <c r="B141">
-        <v>0.0365</v>
+        <v>0.3041666666666666</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1516,7 +1516,7 @@
         <v>37138</v>
       </c>
       <c r="B142">
-        <v>0.0343</v>
+        <v>0.2858333333333333</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1524,7 +1524,7 @@
         <v>37165</v>
       </c>
       <c r="B143">
-        <v>0.0226</v>
+        <v>0.1883333333333333</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1532,7 +1532,7 @@
         <v>37196</v>
       </c>
       <c r="B144">
-        <v>0.0218</v>
+        <v>0.1816666666666667</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1540,7 +1540,7 @@
         <v>37228</v>
       </c>
       <c r="B145">
-        <v>0.0185</v>
+        <v>0.1541666666666667</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1548,7 +1548,7 @@
         <v>37258</v>
       </c>
       <c r="B146">
-        <v>0.0173</v>
+        <v>0.1441666666666667</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1556,7 +1556,7 @@
         <v>37288</v>
       </c>
       <c r="B147">
-        <v>0.0169</v>
+        <v>0.1408333333333333</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1564,7 +1564,7 @@
         <v>37316</v>
       </c>
       <c r="B148">
-        <v>0.0178</v>
+        <v>0.1483333333333333</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1572,7 +1572,7 @@
         <v>37347</v>
       </c>
       <c r="B149">
-        <v>0.0179</v>
+        <v>0.1491666666666667</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1580,7 +1580,7 @@
         <v>37377</v>
       </c>
       <c r="B150">
-        <v>0.0176</v>
+        <v>0.1466666666666667</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1588,7 +1588,7 @@
         <v>37410</v>
       </c>
       <c r="B151">
-        <v>0.0172</v>
+        <v>0.1433333333333333</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1596,7 +1596,7 @@
         <v>37438</v>
       </c>
       <c r="B152">
-        <v>0.0171</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1604,7 +1604,7 @@
         <v>37469</v>
       </c>
       <c r="B153">
-        <v>0.017</v>
+        <v>0.1416666666666667</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1612,7 +1612,7 @@
         <v>37502</v>
       </c>
       <c r="B154">
-        <v>0.0169</v>
+        <v>0.1408333333333333</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1620,7 +1620,7 @@
         <v>37530</v>
       </c>
       <c r="B155">
-        <v>0.0163</v>
+        <v>0.1358333333333333</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1628,7 +1628,7 @@
         <v>37561</v>
       </c>
       <c r="B156">
-        <v>0.0144</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1636,7 +1636,7 @@
         <v>37592</v>
       </c>
       <c r="B157">
-        <v>0.0126</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1644,7 +1644,7 @@
         <v>37623</v>
       </c>
       <c r="B158">
-        <v>0.0118</v>
+        <v>0.09833333333333333</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1652,7 +1652,7 @@
         <v>37655</v>
       </c>
       <c r="B159">
-        <v>0.0116</v>
+        <v>0.09666666666666666</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1660,7 +1660,7 @@
         <v>37683</v>
       </c>
       <c r="B160">
-        <v>0.012</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1668,7 +1668,7 @@
         <v>37712</v>
       </c>
       <c r="B161">
-        <v>0.0117</v>
+        <v>0.09749999999999999</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1676,7 +1676,7 @@
         <v>37742</v>
       </c>
       <c r="B162">
-        <v>0.0109</v>
+        <v>0.09083333333333334</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1684,7 +1684,7 @@
         <v>37774</v>
       </c>
       <c r="B163">
-        <v>0.0117</v>
+        <v>0.09749999999999999</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1692,7 +1692,7 @@
         <v>37803</v>
       </c>
       <c r="B164">
-        <v>0.0089</v>
+        <v>0.07416666666666666</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1700,7 +1700,7 @@
         <v>37834</v>
       </c>
       <c r="B165">
-        <v>0.0091</v>
+        <v>0.07583333333333334</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1708,7 +1708,7 @@
         <v>37866</v>
       </c>
       <c r="B166">
-        <v>0.0098</v>
+        <v>0.08166666666666667</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1716,7 +1716,7 @@
         <v>37895</v>
       </c>
       <c r="B167">
-        <v>0.008800000000000001</v>
+        <v>0.07333333333333333</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1724,7 +1724,7 @@
         <v>37928</v>
       </c>
       <c r="B168">
-        <v>0.0097</v>
+        <v>0.08083333333333333</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1732,7 +1732,7 @@
         <v>37956</v>
       </c>
       <c r="B169">
-        <v>0.009599999999999999</v>
+        <v>0.07999999999999999</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1740,7 +1740,7 @@
         <v>37988</v>
       </c>
       <c r="B170">
-        <v>0.008800000000000001</v>
+        <v>0.07333333333333333</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1748,7 +1748,7 @@
         <v>38019</v>
       </c>
       <c r="B171">
-        <v>0.008699999999999999</v>
+        <v>0.07250000000000001</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1756,7 +1756,7 @@
         <v>38047</v>
       </c>
       <c r="B172">
-        <v>0.0097</v>
+        <v>0.08083333333333333</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1764,7 +1764,7 @@
         <v>38078</v>
       </c>
       <c r="B173">
-        <v>0.0095</v>
+        <v>0.07916666666666666</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1772,7 +1772,7 @@
         <v>38110</v>
       </c>
       <c r="B174">
-        <v>0.0083</v>
+        <v>0.06916666666666667</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1780,7 +1780,7 @@
         <v>38139</v>
       </c>
       <c r="B175">
-        <v>0.0097</v>
+        <v>0.08083333333333333</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1788,7 +1788,7 @@
         <v>38169</v>
       </c>
       <c r="B176">
-        <v>0.0101</v>
+        <v>0.08416666666666667</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1796,7 +1796,7 @@
         <v>38201</v>
       </c>
       <c r="B177">
-        <v>0.0128</v>
+        <v>0.1066666666666667</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1804,7 +1804,7 @@
         <v>38231</v>
       </c>
       <c r="B178">
-        <v>0.0143</v>
+        <v>0.1191666666666667</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1812,7 +1812,7 @@
         <v>38261</v>
       </c>
       <c r="B179">
-        <v>0.0152</v>
+        <v>0.1266666666666667</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1820,7 +1820,7 @@
         <v>38292</v>
       </c>
       <c r="B180">
-        <v>0.0179</v>
+        <v>0.1491666666666667</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1828,7 +1828,7 @@
         <v>38322</v>
       </c>
       <c r="B181">
-        <v>0.0206</v>
+        <v>0.1716666666666667</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1836,7 +1836,7 @@
         <v>38355</v>
       </c>
       <c r="B182">
-        <v>0.0199</v>
+        <v>0.1658333333333333</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1844,7 +1844,7 @@
         <v>38384</v>
       </c>
       <c r="B183">
-        <v>0.0223</v>
+        <v>0.1858333333333334</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1852,7 +1852,7 @@
         <v>38412</v>
       </c>
       <c r="B184">
-        <v>0.0255</v>
+        <v>0.2125</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1860,7 +1860,7 @@
         <v>38443</v>
       </c>
       <c r="B185">
-        <v>0.0266</v>
+        <v>0.2216666666666667</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1868,7 +1868,7 @@
         <v>38474</v>
       </c>
       <c r="B186">
-        <v>0.0268</v>
+        <v>0.2233333333333334</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1876,7 +1876,7 @@
         <v>38504</v>
       </c>
       <c r="B187">
-        <v>0.0279</v>
+        <v>0.2325</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1884,7 +1884,7 @@
         <v>38534</v>
       </c>
       <c r="B188">
-        <v>0.0302</v>
+        <v>0.2516666666666666</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1892,7 +1892,7 @@
         <v>38565</v>
       </c>
       <c r="B189">
-        <v>0.033</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1900,7 +1900,7 @@
         <v>38596</v>
       </c>
       <c r="B190">
-        <v>0.0335</v>
+        <v>0.2791666666666667</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1908,7 +1908,7 @@
         <v>38628</v>
       </c>
       <c r="B191">
-        <v>0.0322</v>
+        <v>0.2683333333333334</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1916,7 +1916,7 @@
         <v>38657</v>
       </c>
       <c r="B192">
-        <v>0.0378</v>
+        <v>0.315</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1924,7 +1924,7 @@
         <v>38687</v>
       </c>
       <c r="B193">
-        <v>0.0399</v>
+        <v>0.3325</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1932,7 +1932,7 @@
         <v>38720</v>
       </c>
       <c r="B194">
-        <v>0.0405</v>
+        <v>0.3375</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1940,7 +1940,7 @@
         <v>38749</v>
       </c>
       <c r="B195">
-        <v>0.0433</v>
+        <v>0.3608333333333333</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1948,7 +1948,7 @@
         <v>38777</v>
       </c>
       <c r="B196">
-        <v>0.0445</v>
+        <v>0.3708333333333333</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1956,7 +1956,7 @@
         <v>38810</v>
       </c>
       <c r="B197">
-        <v>0.0466</v>
+        <v>0.3883333333333334</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1964,7 +1964,7 @@
         <v>38838</v>
       </c>
       <c r="B198">
-        <v>0.0461</v>
+        <v>0.3841666666666667</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1972,7 +1972,7 @@
         <v>38869</v>
       </c>
       <c r="B199">
-        <v>0.0475</v>
+        <v>0.3958333333333333</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1980,7 +1980,7 @@
         <v>38901</v>
       </c>
       <c r="B200">
-        <v>0.0469</v>
+        <v>0.3908333333333334</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1988,7 +1988,7 @@
         <v>38930</v>
       </c>
       <c r="B201">
-        <v>0.052</v>
+        <v>0.4333333333333333</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -1996,7 +1996,7 @@
         <v>38961</v>
       </c>
       <c r="B202">
-        <v>0.0507</v>
+        <v>0.4225</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2004,7 +2004,7 @@
         <v>38992</v>
       </c>
       <c r="B203">
-        <v>0.0467</v>
+        <v>0.3891666666666667</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2012,7 +2012,7 @@
         <v>39022</v>
       </c>
       <c r="B204">
-        <v>0.0519</v>
+        <v>0.4325000000000001</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2020,7 +2020,7 @@
         <v>39052</v>
       </c>
       <c r="B205">
-        <v>0.0521</v>
+        <v>0.4341666666666667</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2028,7 +2028,7 @@
         <v>39084</v>
       </c>
       <c r="B206">
-        <v>0.0479</v>
+        <v>0.3991666666666666</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2036,7 +2036,7 @@
         <v>39114</v>
       </c>
       <c r="B207">
-        <v>0.0499</v>
+        <v>0.4158333333333334</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2044,7 +2044,7 @@
         <v>39142</v>
       </c>
       <c r="B208">
-        <v>0.0525</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2052,7 +2052,7 @@
         <v>39174</v>
       </c>
       <c r="B209">
-        <v>0.0512</v>
+        <v>0.4266666666666666</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2060,7 +2060,7 @@
         <v>39203</v>
       </c>
       <c r="B210">
-        <v>0.0469</v>
+        <v>0.3908333333333334</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2068,7 +2068,7 @@
         <v>39234</v>
       </c>
       <c r="B211">
-        <v>0.048</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2076,7 +2076,7 @@
         <v>39265</v>
       </c>
       <c r="B212">
-        <v>0.0455</v>
+        <v>0.3791666666666667</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2084,7 +2084,7 @@
         <v>39295</v>
       </c>
       <c r="B213">
-        <v>0.0505</v>
+        <v>0.4208333333333333</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2092,7 +2092,7 @@
         <v>39329</v>
       </c>
       <c r="B214">
-        <v>0.0455</v>
+        <v>0.3791666666666667</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2100,7 +2100,7 @@
         <v>39356</v>
       </c>
       <c r="B215">
-        <v>0.0352</v>
+        <v>0.2933333333333333</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2108,7 +2108,7 @@
         <v>39387</v>
       </c>
       <c r="B216">
-        <v>0.039</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2116,7 +2116,7 @@
         <v>39419</v>
       </c>
       <c r="B217">
-        <v>0.0355</v>
+        <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2124,7 +2124,7 @@
         <v>39449</v>
       </c>
       <c r="B218">
-        <v>0.0309</v>
+        <v>0.2575</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2132,7 +2132,7 @@
         <v>39479</v>
       </c>
       <c r="B219">
-        <v>0.0175</v>
+        <v>0.1458333333333333</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2140,7 +2140,7 @@
         <v>39510</v>
       </c>
       <c r="B220">
-        <v>0.0199</v>
+        <v>0.1658333333333333</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2148,7 +2148,7 @@
         <v>39539</v>
       </c>
       <c r="B221">
-        <v>0.0155</v>
+        <v>0.1291666666666667</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2156,7 +2156,7 @@
         <v>39569</v>
       </c>
       <c r="B222">
-        <v>0.0123</v>
+        <v>0.1025</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2164,7 +2164,7 @@
         <v>39601</v>
       </c>
       <c r="B223">
-        <v>0.0194</v>
+        <v>0.1616666666666667</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2172,7 +2172,7 @@
         <v>39630</v>
       </c>
       <c r="B224">
-        <v>0.0192</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2180,7 +2180,7 @@
         <v>39661</v>
       </c>
       <c r="B225">
-        <v>0.0152</v>
+        <v>0.1266666666666667</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2188,7 +2188,7 @@
         <v>39693</v>
       </c>
       <c r="B226">
-        <v>0.0164</v>
+        <v>0.1366666666666667</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2196,7 +2196,7 @@
         <v>39722</v>
       </c>
       <c r="B227">
-        <v>0.0066</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2204,7 +2204,7 @@
         <v>39755</v>
       </c>
       <c r="B228">
-        <v>0.002</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2212,7 +2212,7 @@
         <v>39783</v>
       </c>
       <c r="B229">
-        <v>0.0009</v>
+        <v>0.007499999999999999</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2220,7 +2220,7 @@
         <v>39815</v>
       </c>
       <c r="B230">
-        <v>0.0004</v>
+        <v>0.003333333333333333</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2228,7 +2228,7 @@
         <v>39846</v>
       </c>
       <c r="B231">
-        <v>0.0019</v>
+        <v>0.01583333333333333</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2236,7 +2236,7 @@
         <v>39874</v>
       </c>
       <c r="B232">
-        <v>0.0017</v>
+        <v>0.01416666666666667</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2244,7 +2244,7 @@
         <v>39904</v>
       </c>
       <c r="B233">
-        <v>0.0018</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2252,7 +2252,7 @@
         <v>39934</v>
       </c>
       <c r="B234">
-        <v>0.0005999999999999999</v>
+        <v>0.004999999999999999</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2260,7 +2260,7 @@
         <v>39965</v>
       </c>
       <c r="B235">
-        <v>0.0013</v>
+        <v>0.01083333333333333</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2268,7 +2268,7 @@
         <v>39995</v>
       </c>
       <c r="B236">
-        <v>0.0013</v>
+        <v>0.01083333333333333</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2276,7 +2276,7 @@
         <v>40028</v>
       </c>
       <c r="B237">
-        <v>0.0015</v>
+        <v>0.0125</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2284,7 +2284,7 @@
         <v>40057</v>
       </c>
       <c r="B238">
-        <v>0.0008</v>
+        <v>0.006666666666666666</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2292,7 +2292,7 @@
         <v>40087</v>
       </c>
       <c r="B239">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2300,7 +2300,7 @@
         <v>40119</v>
       </c>
       <c r="B240">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2308,7 +2308,7 @@
         <v>40148</v>
       </c>
       <c r="B241">
-        <v>0.0009</v>
+        <v>0.007499999999999999</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2316,7 +2316,7 @@
         <v>40182</v>
       </c>
       <c r="B242">
-        <v>0.0005</v>
+        <v>0.004166666666666667</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2324,7 +2324,7 @@
         <v>40210</v>
       </c>
       <c r="B243">
-        <v>0.0005</v>
+        <v>0.004166666666666667</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2332,7 +2332,7 @@
         <v>40238</v>
       </c>
       <c r="B244">
-        <v>0.0009</v>
+        <v>0.007499999999999999</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2340,7 +2340,7 @@
         <v>40269</v>
       </c>
       <c r="B245">
-        <v>0.0016</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2348,7 +2348,7 @@
         <v>40301</v>
       </c>
       <c r="B246">
-        <v>0.0014</v>
+        <v>0.01166666666666667</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2356,7 +2356,7 @@
         <v>40330</v>
       </c>
       <c r="B247">
-        <v>0.0014</v>
+        <v>0.01166666666666667</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2364,7 +2364,7 @@
         <v>40360</v>
       </c>
       <c r="B248">
-        <v>0.0016</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2372,7 +2372,7 @@
         <v>40392</v>
       </c>
       <c r="B249">
-        <v>0.0014</v>
+        <v>0.01166666666666667</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2380,7 +2380,7 @@
         <v>40422</v>
       </c>
       <c r="B250">
-        <v>0.0016</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2388,7 +2388,7 @@
         <v>40452</v>
       </c>
       <c r="B251">
-        <v>0.0015</v>
+        <v>0.0125</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2396,7 +2396,7 @@
         <v>40483</v>
       </c>
       <c r="B252">
-        <v>0.0014</v>
+        <v>0.01166666666666667</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2404,7 +2404,7 @@
         <v>40513</v>
       </c>
       <c r="B253">
-        <v>0.0017</v>
+        <v>0.01416666666666667</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2412,7 +2412,7 @@
         <v>40546</v>
       </c>
       <c r="B254">
-        <v>0.0011</v>
+        <v>0.009166666666666667</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2420,7 +2420,7 @@
         <v>40575</v>
       </c>
       <c r="B255">
-        <v>0.0016</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2428,7 +2428,7 @@
         <v>40603</v>
       </c>
       <c r="B256">
-        <v>0.0007000000000000001</v>
+        <v>0.005833333333333334</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2436,7 +2436,7 @@
         <v>40634</v>
       </c>
       <c r="B257">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2444,7 +2444,7 @@
         <v>40665</v>
       </c>
       <c r="B258">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2452,7 +2452,7 @@
         <v>40695</v>
       </c>
       <c r="B259">
-        <v>0.0004</v>
+        <v>0.003333333333333333</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2460,7 +2460,7 @@
         <v>40725</v>
       </c>
       <c r="B260">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2468,7 +2468,7 @@
         <v>40756</v>
       </c>
       <c r="B261">
-        <v>0.0013</v>
+        <v>0.01083333333333333</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2476,7 +2476,7 @@
         <v>40787</v>
       </c>
       <c r="B262">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2484,7 +2484,7 @@
         <v>40819</v>
       </c>
       <c r="B263">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2492,7 +2492,7 @@
         <v>40848</v>
       </c>
       <c r="B264">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2500,7 +2500,7 @@
         <v>40878</v>
       </c>
       <c r="B265">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2508,7 +2508,7 @@
         <v>40911</v>
       </c>
       <c r="B266">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2516,7 +2516,7 @@
         <v>40940</v>
       </c>
       <c r="B267">
-        <v>0.0005</v>
+        <v>0.004166666666666667</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2524,7 +2524,7 @@
         <v>40969</v>
       </c>
       <c r="B268">
-        <v>0.0007000000000000001</v>
+        <v>0.005833333333333334</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2532,7 +2532,7 @@
         <v>41001</v>
       </c>
       <c r="B269">
-        <v>0.0005</v>
+        <v>0.004166666666666667</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2540,7 +2540,7 @@
         <v>41030</v>
       </c>
       <c r="B270">
-        <v>0.0007000000000000001</v>
+        <v>0.005833333333333334</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2548,7 +2548,7 @@
         <v>41061</v>
       </c>
       <c r="B271">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2556,7 +2556,7 @@
         <v>41092</v>
       </c>
       <c r="B272">
-        <v>0.0005999999999999999</v>
+        <v>0.004999999999999999</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2564,7 +2564,7 @@
         <v>41122</v>
       </c>
       <c r="B273">
-        <v>0.0007000000000000001</v>
+        <v>0.005833333333333334</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2572,7 +2572,7 @@
         <v>41156</v>
       </c>
       <c r="B274">
-        <v>0.001</v>
+        <v>0.008333333333333333</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2580,7 +2580,7 @@
         <v>41183</v>
       </c>
       <c r="B275">
-        <v>0.0005</v>
+        <v>0.004166666666666667</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -2588,7 +2588,7 @@
         <v>41214</v>
       </c>
       <c r="B276">
-        <v>0.0005999999999999999</v>
+        <v>0.004999999999999999</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -2596,7 +2596,7 @@
         <v>41246</v>
       </c>
       <c r="B277">
-        <v>0.0013</v>
+        <v>0.01083333333333333</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -2604,7 +2604,7 @@
         <v>41276</v>
       </c>
       <c r="B278">
-        <v>0.0007000000000000001</v>
+        <v>0.005833333333333334</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2612,7 +2612,7 @@
         <v>41306</v>
       </c>
       <c r="B279">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2620,7 +2620,7 @@
         <v>41334</v>
       </c>
       <c r="B280">
-        <v>0.0007000000000000001</v>
+        <v>0.005833333333333334</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2628,7 +2628,7 @@
         <v>41365</v>
       </c>
       <c r="B281">
-        <v>0.0005999999999999999</v>
+        <v>0.004999999999999999</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2636,7 +2636,7 @@
         <v>41395</v>
       </c>
       <c r="B282">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2644,7 +2644,7 @@
         <v>41428</v>
       </c>
       <c r="B283">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2652,7 +2652,7 @@
         <v>41456</v>
       </c>
       <c r="B284">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2660,7 +2660,7 @@
         <v>41487</v>
       </c>
       <c r="B285">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2668,7 +2668,7 @@
         <v>41520</v>
       </c>
       <c r="B286">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2676,7 +2676,7 @@
         <v>41548</v>
       </c>
       <c r="B287">
-        <v>0.001</v>
+        <v>0.008333333333333333</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2684,7 +2684,7 @@
         <v>41579</v>
       </c>
       <c r="B288">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2692,7 +2692,7 @@
         <v>41610</v>
       </c>
       <c r="B289">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2700,7 +2700,7 @@
         <v>41641</v>
       </c>
       <c r="B290">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -2708,7 +2708,7 @@
         <v>41673</v>
       </c>
       <c r="B291">
-        <v>0.0004</v>
+        <v>0.003333333333333333</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2716,7 +2716,7 @@
         <v>41701</v>
       </c>
       <c r="B292">
-        <v>0.0004</v>
+        <v>0.003333333333333333</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -2724,7 +2724,7 @@
         <v>41730</v>
       </c>
       <c r="B293">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2732,7 +2732,7 @@
         <v>41760</v>
       </c>
       <c r="B294">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2740,7 +2740,7 @@
         <v>41792</v>
       </c>
       <c r="B295">
-        <v>0.0004</v>
+        <v>0.003333333333333333</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2748,7 +2748,7 @@
         <v>41821</v>
       </c>
       <c r="B296">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2756,7 +2756,7 @@
         <v>41852</v>
       </c>
       <c r="B297">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2764,7 +2764,7 @@
         <v>41884</v>
       </c>
       <c r="B298">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2772,7 +2772,7 @@
         <v>41913</v>
       </c>
       <c r="B299">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2780,7 +2780,7 @@
         <v>41946</v>
       </c>
       <c r="B300">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2788,7 +2788,7 @@
         <v>41974</v>
       </c>
       <c r="B301">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2796,7 +2796,7 @@
         <v>42006</v>
       </c>
       <c r="B302">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2804,7 +2804,7 @@
         <v>42037</v>
       </c>
       <c r="B303">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2812,7 +2812,7 @@
         <v>42065</v>
       </c>
       <c r="B304">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2820,7 +2820,7 @@
         <v>42095</v>
       </c>
       <c r="B305">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2836,7 +2836,7 @@
         <v>42156</v>
       </c>
       <c r="B307">
-        <v>0.0002</v>
+        <v>0.001666666666666667</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2844,7 +2844,7 @@
         <v>42186</v>
       </c>
       <c r="B308">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2852,7 +2852,7 @@
         <v>42219</v>
       </c>
       <c r="B309">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2860,7 +2860,7 @@
         <v>42248</v>
       </c>
       <c r="B310">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2876,7 +2876,7 @@
         <v>42310</v>
       </c>
       <c r="B312">
-        <v>0.0001</v>
+        <v>0.0008333333333333333</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2884,7 +2884,7 @@
         <v>42339</v>
       </c>
       <c r="B313">
-        <v>0.0019</v>
+        <v>0.01583333333333333</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2892,7 +2892,7 @@
         <v>42373</v>
       </c>
       <c r="B314">
-        <v>0.0017</v>
+        <v>0.01416666666666667</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2900,7 +2900,7 @@
         <v>42401</v>
       </c>
       <c r="B315">
-        <v>0.0019</v>
+        <v>0.01583333333333333</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2908,7 +2908,7 @@
         <v>42430</v>
       </c>
       <c r="B316">
-        <v>0.0029</v>
+        <v>0.02416666666666667</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2916,7 +2916,7 @@
         <v>42461</v>
       </c>
       <c r="B317">
-        <v>0.002</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2924,7 +2924,7 @@
         <v>42492</v>
       </c>
       <c r="B318">
-        <v>0.0011</v>
+        <v>0.009166666666666667</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2932,7 +2932,7 @@
         <v>42522</v>
       </c>
       <c r="B319">
-        <v>0.0027</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2940,7 +2940,7 @@
         <v>42552</v>
       </c>
       <c r="B320">
-        <v>0.0024</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2948,7 +2948,7 @@
         <v>42583</v>
       </c>
       <c r="B321">
-        <v>0.002</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2956,7 +2956,7 @@
         <v>42614</v>
       </c>
       <c r="B322">
-        <v>0.0027</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2964,7 +2964,7 @@
         <v>42646</v>
       </c>
       <c r="B323">
-        <v>0.0025</v>
+        <v>0.02083333333333333</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2972,7 +2972,7 @@
         <v>42675</v>
       </c>
       <c r="B324">
-        <v>0.0024</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2980,7 +2980,7 @@
         <v>42705</v>
       </c>
       <c r="B325">
-        <v>0.0032</v>
+        <v>0.02666666666666666</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -2988,7 +2988,7 @@
         <v>42738</v>
       </c>
       <c r="B326">
-        <v>0.0052</v>
+        <v>0.04333333333333333</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -2996,7 +2996,7 @@
         <v>42767</v>
       </c>
       <c r="B327">
-        <v>0.005</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -3004,7 +3004,7 @@
         <v>42795</v>
       </c>
       <c r="B328">
-        <v>0.0046</v>
+        <v>0.03833333333333334</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -3012,7 +3012,7 @@
         <v>42828</v>
       </c>
       <c r="B329">
-        <v>0.0073</v>
+        <v>0.06083333333333333</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3020,7 +3020,7 @@
         <v>42856</v>
       </c>
       <c r="B330">
-        <v>0.0067</v>
+        <v>0.05583333333333334</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3028,7 +3028,7 @@
         <v>42887</v>
       </c>
       <c r="B331">
-        <v>0.008199999999999999</v>
+        <v>0.06833333333333333</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3036,7 +3036,7 @@
         <v>42919</v>
       </c>
       <c r="B332">
-        <v>0.009599999999999999</v>
+        <v>0.07999999999999999</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3044,7 +3044,7 @@
         <v>42948</v>
       </c>
       <c r="B333">
-        <v>0.01</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3052,7 +3052,7 @@
         <v>42979</v>
       </c>
       <c r="B334">
-        <v>0.009599999999999999</v>
+        <v>0.07999999999999999</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3060,7 +3060,7 @@
         <v>43010</v>
       </c>
       <c r="B335">
-        <v>0.0095</v>
+        <v>0.07916666666666666</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3068,7 +3068,7 @@
         <v>43040</v>
       </c>
       <c r="B336">
-        <v>0.0106</v>
+        <v>0.08833333333333333</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3076,7 +3076,7 @@
         <v>43070</v>
       </c>
       <c r="B337">
-        <v>0.0114</v>
+        <v>0.09499999999999999</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3084,7 +3084,7 @@
         <v>43102</v>
       </c>
       <c r="B338">
-        <v>0.0129</v>
+        <v>0.1075</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3092,7 +3092,7 @@
         <v>43132</v>
       </c>
       <c r="B339">
-        <v>0.0141</v>
+        <v>0.1175</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3100,7 +3100,7 @@
         <v>43160</v>
       </c>
       <c r="B340">
-        <v>0.015</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3108,7 +3108,7 @@
         <v>43192</v>
       </c>
       <c r="B341">
-        <v>0.0168</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3116,7 +3116,7 @@
         <v>43221</v>
       </c>
       <c r="B342">
-        <v>0.0168</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3124,7 +3124,7 @@
         <v>43252</v>
       </c>
       <c r="B343">
-        <v>0.0174</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3132,7 +3132,7 @@
         <v>43283</v>
       </c>
       <c r="B344">
-        <v>0.019</v>
+        <v>0.1583333333333333</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3140,7 +3140,7 @@
         <v>43313</v>
       </c>
       <c r="B345">
-        <v>0.0193</v>
+        <v>0.1608333333333333</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3148,7 +3148,7 @@
         <v>43347</v>
       </c>
       <c r="B346">
-        <v>0.02</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3156,7 +3156,7 @@
         <v>43374</v>
       </c>
       <c r="B347">
-        <v>0.0213</v>
+        <v>0.1775</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3164,7 +3164,7 @@
         <v>43405</v>
       </c>
       <c r="B348">
-        <v>0.0221</v>
+        <v>0.1841666666666666</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3172,7 +3172,7 @@
         <v>43437</v>
       </c>
       <c r="B349">
-        <v>0.023</v>
+        <v>0.1916666666666667</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3180,7 +3180,7 @@
         <v>43467</v>
       </c>
       <c r="B350">
-        <v>0.024</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3188,7 +3188,7 @@
         <v>43497</v>
       </c>
       <c r="B351">
-        <v>0.0241</v>
+        <v>0.2008333333333334</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3196,7 +3196,7 @@
         <v>43525</v>
       </c>
       <c r="B352">
-        <v>0.0244</v>
+        <v>0.2033333333333333</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3204,7 +3204,7 @@
         <v>43556</v>
       </c>
       <c r="B353">
-        <v>0.0242</v>
+        <v>0.2016666666666667</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3212,7 +3212,7 @@
         <v>43586</v>
       </c>
       <c r="B354">
-        <v>0.0242</v>
+        <v>0.2016666666666667</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3220,7 +3220,7 @@
         <v>43619</v>
       </c>
       <c r="B355">
-        <v>0.0236</v>
+        <v>0.1966666666666667</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3228,7 +3228,7 @@
         <v>43647</v>
       </c>
       <c r="B356">
-        <v>0.0217</v>
+        <v>0.1808333333333333</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3236,7 +3236,7 @@
         <v>43678</v>
       </c>
       <c r="B357">
-        <v>0.0211</v>
+        <v>0.1758333333333333</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3244,7 +3244,7 @@
         <v>43711</v>
       </c>
       <c r="B358">
-        <v>0.0206</v>
+        <v>0.1716666666666667</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3252,7 +3252,7 @@
         <v>43739</v>
       </c>
       <c r="B359">
-        <v>0.0179</v>
+        <v>0.1491666666666667</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3260,7 +3260,7 @@
         <v>43770</v>
       </c>
       <c r="B360">
-        <v>0.0158</v>
+        <v>0.1316666666666667</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3268,7 +3268,7 @@
         <v>43801</v>
       </c>
       <c r="B361">
-        <v>0.016</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3276,7 +3276,7 @@
         <v>43832</v>
       </c>
       <c r="B362">
-        <v>0.0153</v>
+        <v>0.1275</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3284,7 +3284,7 @@
         <v>43864</v>
       </c>
       <c r="B363">
-        <v>0.0156</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3292,7 +3292,7 @@
         <v>43892</v>
       </c>
       <c r="B364">
-        <v>0.0141</v>
+        <v>0.1175</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3300,7 +3300,7 @@
         <v>43922</v>
       </c>
       <c r="B365">
-        <v>0.0003</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3308,7 +3308,7 @@
         <v>43952</v>
       </c>
       <c r="B366">
-        <v>0.001</v>
+        <v>0.008333333333333333</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3316,7 +3316,7 @@
         <v>43983</v>
       </c>
       <c r="B367">
-        <v>0.0012</v>
+        <v>0.009999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>